<commit_message>
Ticket 48 - When determining how much content to shift out of the way, consider cells that may be blank but still contain styling (CellStyle's index isn't the default 0).
</commit_message>
<xml_diff>
--- a/jett-core/templates/ForTagTemplate.xlsx
+++ b/jett-core/templates/ForTagTemplate.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Multiplication" sheetId="1" r:id="rId1"/>
     <sheet name="OneOrZero" sheetId="2" r:id="rId2"/>
     <sheet name="End" sheetId="3" r:id="rId3"/>
+    <sheet name="Immaterial" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>X</t>
   </si>
@@ -81,12 +82,24 @@
   <si>
     <t>${y % 3 == 0}&lt;/jt:for&gt;</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>&lt;jt:for start="10" end="0" step="-2" var="n"&gt;${n}</t>
+  </si>
+  <si>
+    <t>${n * n}&lt;/jt:for&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +131,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +155,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,13 +198,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,4 +632,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>